<commit_message>
Rapport: presentation resultats et discussion
</commit_message>
<xml_diff>
--- a/rapport/resultats.xlsx
+++ b/rapport/resultats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Centre de masse</t>
   </si>
@@ -128,10 +128,6 @@
   <si>
     <t>Bras gauche 
 ⏊ au tronc</t>
-  </si>
-  <si>
-    <t>Bras gauche 
-⏊e au tronc</t>
   </si>
   <si>
     <t>Config.\ Question</t>
@@ -773,7 +769,7 @@
   <dimension ref="B1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,7 +787,7 @@
         <v>21</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>2</v>
@@ -816,10 +812,10 @@
         <v>1</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -883,7 +879,7 @@
     <row r="7" spans="2:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7"/>
       <c r="C7" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>17</v>

</xml_diff>